<commit_message>
Se ponen los comentarios linea a linea para saber que hace cada instruccion
</commit_message>
<xml_diff>
--- a/validacion.xlsx
+++ b/validacion.xlsx
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1073,6 +1073,62 @@
         <v>10525717.85</v>
       </c>
     </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>20000000</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13" si="12">0.04*A13 *B13</f>
+        <v>800000</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13" si="13">0.045*A13*B13</f>
+        <v>900000</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13" si="14">0.04*A13*B13</f>
+        <v>800000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13" si="15">0.08*A13*B13</f>
+        <v>1600000</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="16">A13-C13/B13-E13/B13-H13/B13+IF(A13/$B$2 &lt;= 2, $A$2, 0)</f>
+        <v>18000000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13" si="17">A13*L13*B13</f>
+        <v>400000</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13" si="18">A13-C13/B13-E13/B13-H13/B13</f>
+        <v>18000000</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13" si="19">(I13-I13*0.25)*B13</f>
+        <v>13500000</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13" si="20">B13 * IF(AND(M13 &gt; 0, M13 &lt;= 95),0,IF(AND(M13 &gt; 95, M13 &lt;= 150),((M13 - 95)*$C$2)*0.19,IF(AND(M13 &gt; 150, M13 &lt;= 360),((M13 - 150)*$C$2)*0.28 + 10*$C$2,((M13 - 360)*$C$2)*0.33 + 69*$C$2)))</f>
+        <v>3046705.8</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13" si="21">IF(A13/$B$2&lt;4,0,IF(AND(A13/$B$2&gt;=4,A13/$B$2&lt;16),$D$2,IF(AND(A13/$B$2&gt;=16,A13/$B$2&lt;17),$E$2,IF(AND(A13/$B$2&gt;=17,A13/$B$2&lt;18),$F$2,IF(AND(A13/$B$2&gt;=18,A13/$B$2&lt;19),$G$2,IF(AND(A13/$B$2&gt;=19,A13/$B$2&lt;20),$H$2,$I$2))))))</f>
+        <v>0.02</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13" si="22">(J13/B13)/$C$2</f>
+        <v>477.38604618267971</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13" si="23">G13 * B13-(K13/B13)</f>
+        <v>14953294.199999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Adding tests to the excel document
</commit_message>
<xml_diff>
--- a/validacion.xlsx
+++ b/validacion.xlsx
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1129,6 +1129,63 @@
         <v>14953294.199999999</v>
       </c>
     </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <f>2.5*B4</f>
+        <v>1610875</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14" si="24">0.04*A14 *B14</f>
+        <v>64435</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="25">0.045*A14*B14</f>
+        <v>72489.375</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="26">0.04*A14*B14</f>
+        <v>64435</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14" si="27">0.08*A14*B14</f>
+        <v>128870</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="28">A14-C14/B14-E14/B14-H14/B14+IF(A14/$B$2 &lt;= 2, $A$2, 0)</f>
+        <v>1482005</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14" si="29">A14*L14*B14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14" si="30">A14-C14/B14-E14/B14-H14/B14</f>
+        <v>1482005</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14" si="31">(I14-I14*0.25)*B14</f>
+        <v>1111503.75</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14" si="32">B14 * IF(AND(M14 &gt; 0, M14 &lt;= 95),0,IF(AND(M14 &gt; 95, M14 &lt;= 150),((M14 - 95)*$C$2)*0.19,IF(AND(M14 &gt; 150, M14 &lt;= 360),((M14 - 150)*$C$2)*0.28 + 10*$C$2,((M14 - 360)*$C$2)*0.33 + 69*$C$2)))</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14" si="33">IF(A14/$B$2&lt;4,0,IF(AND(A14/$B$2&gt;=4,A14/$B$2&lt;16),$D$2,IF(AND(A14/$B$2&gt;=16,A14/$B$2&lt;17),$E$2,IF(AND(A14/$B$2&gt;=17,A14/$B$2&lt;18),$F$2,IF(AND(A14/$B$2&gt;=18,A14/$B$2&lt;19),$G$2,IF(AND(A14/$B$2&gt;=19,A14/$B$2&lt;20),$H$2,$I$2))))))</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14" si="34">(J14/B14)/$C$2</f>
+        <v>39.304917076275679</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14" si="35">G14 * B14-(K14/B14)</f>
+        <v>1482005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>